<commit_message>
fix: add sumitter role to hmd submission class
</commit_message>
<xml_diff>
--- a/Formulasation(shacl)/core/Templates/SHACL-hmd-submission.xlsx
+++ b/Formulasation(shacl)/core/Templates/SHACL-hmd-submission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/gdi-metadata/Formulasation(shacl)/core/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{67D697DE-5446-C941-BDB7-13D5AA62327A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF012941-D602-4AE9-AA08-88DB5B6871BC}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="13_ncr:1_{67D697DE-5446-C941-BDB7-13D5AA62327A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CF37916-B06B-4BF8-927E-532715D75E61}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="168">
   <si>
     <t>PREFIX</t>
   </si>
@@ -536,6 +536,15 @@
   </si>
   <si>
     <t>http://data.health-ri.nl/GDI/HMDSubmissionShape</t>
+  </si>
+  <si>
+    <t>Submitter Role</t>
+  </si>
+  <si>
+    <t>Role of the Submitter (e.g. Oncologist in charge of the patient, Research Project PI).</t>
+  </si>
+  <si>
+    <t>fg:0000752</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2352,7 @@
       </c>
       <c r="B7" s="6">
         <f ca="1">NOW()</f>
-        <v>45849.491382986111</v>
+        <v>45849.497614004627</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -2498,12 +2507,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="E13" sqref="E13"/>
-      <selection pane="topRight" activeCell="B14" sqref="B14"/>
+      <selection pane="topRight" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2740,7 +2749,7 @@
     </row>
     <row r="9" spans="1:25" s="66" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="str">
-        <f t="shared" ref="A9:A15" si="0">CONCATENATE(B9,"#",C9)</f>
+        <f t="shared" ref="A9:A16" si="0">CONCATENATE(B9,"#",C9)</f>
         <v>gdi:HMDsubmissionShape#fg:0000753</v>
       </c>
       <c r="B9" s="67" t="s">
@@ -2974,6 +2983,33 @@
         <v>132</v>
       </c>
       <c r="Y15" s="73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="str">
+        <f t="shared" si="0"/>
+        <v>gdi:HMDsubmissionShape#fg:0000752</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="X16" s="64" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y16" s="64" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3005,6 +3041,36 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+    <Persoon xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Persoon>
+    <Opmerkingen xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31f6c59cfd598d1d7de5b45c1822abcd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67714481eaab3d0eef8b708c465ce66d" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -3292,37 +3358,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFAAEB16-68DD-4D0B-ABEE-F5FFA1FFD6CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <Categorie xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-    <Persoon xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Persoon>
-    <Opmerkingen xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF0D4BE-F0F3-4B03-A8BD-9CD4C60B556D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{228A4FD4-9C74-4788-AC27-9C2192995994}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3339,23 +3394,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF0D4BE-F0F3-4B03-A8BD-9CD4C60B556D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFAAEB16-68DD-4D0B-ABEE-F5FFA1FFD6CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>